<commit_message>
Getting first session correct
</commit_message>
<xml_diff>
--- a/Main notebooks/files/excel_importer_example.xlsx
+++ b/Main notebooks/files/excel_importer_example.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10307"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmutel/Code/Brightway-Seminar-2020/Main notebooks/files/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8A4FB6-4EE1-4545-B852-0C6CFBCA1221}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="0" windowWidth="28300" windowHeight="20520" activeTab="1"/>
+    <workbookView xWindow="500" yWindow="460" windowWidth="28300" windowHeight="17540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="skip this sheet" sheetId="2" r:id="rId1"/>
     <sheet name="first process" sheetId="1" r:id="rId2"/>
     <sheet name="other process" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="58">
   <si>
     <t>Database</t>
   </si>
@@ -189,9 +195,6 @@
   </si>
   <si>
     <t>tap water, at user</t>
-  </si>
-  <si>
-    <t>drunk water</t>
   </si>
   <si>
     <t>WriteSomeCode_UUID_isFineButNotNecessary</t>
@@ -203,10 +206,17 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -255,6 +265,7 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -277,42 +288,43 @@
   </borders>
   <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -644,31 +656,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
@@ -684,14 +696,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="50.6640625" customWidth="1"/>
     <col min="2" max="2" width="24.6640625" customWidth="1"/>
@@ -702,7 +714,7 @@
     <col min="7" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -713,7 +725,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15">
+    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -724,7 +736,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -735,12 +747,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C4" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15">
+    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -751,7 +763,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -759,7 +771,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -767,7 +779,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -775,7 +787,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -783,7 +795,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -791,7 +803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -799,7 +811,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -807,12 +819,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15">
+    <row r="14" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15">
+    <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -850,7 +862,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -861,7 +873,7 @@
         <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E16" t="s">
         <v>46</v>
@@ -888,7 +900,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -899,7 +911,7 @@
         <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E17" t="s">
         <v>46</v>
@@ -926,7 +938,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15">
+    <row r="18" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>48</v>
       </c>
@@ -976,19 +988,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="41.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -996,12 +1008,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15">
+    <row r="4" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1009,7 +1021,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1017,15 +1029,15 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1033,7 +1045,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1041,7 +1053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1049,7 +1061,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1066,7 +1078,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15">
+    <row r="11" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -1080,7 +1092,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="15">
+    <row r="12" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -1118,7 +1130,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15">
+    <row r="13" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>48</v>
       </c>
@@ -1160,7 +1172,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -1171,7 +1183,7 @@
         <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E14" t="s">
         <v>47</v>
@@ -1198,9 +1210,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
-      <c r="A15" t="s">
-        <v>56</v>
+    <row r="15" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1209,7 +1221,7 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E15" t="s">
         <v>47</v>

</xml_diff>